<commit_message>
change controlpanel2 excel file
</commit_message>
<xml_diff>
--- a/ControlPanel2_TestFile2.xlsx
+++ b/ControlPanel2_TestFile2.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false" codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16395" tabRatio="500" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet name="SheetJS" sheetId="1" r:id="rId1"/>
+    <sheet name="personal_information" sheetId="1" r:id="rId1"/>
+    <sheet name="form" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="154">
   <si>
     <t>機號</t>
   </si>
@@ -56,12 +75,75 @@
     <t/>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>08A_21_03</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>Malignant neoplasm of body of pancr...</t>
+  </si>
+  <si>
+    <t>Pancreatico-duodenectomy| Whip</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>葉育彰</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>劉xx</t>
+  </si>
+  <si>
+    <t>08B_07_02</t>
+  </si>
+  <si>
+    <t>2234567</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>Esophageal cancer</t>
+  </si>
+  <si>
+    <t>MIE (Tri-incision)</t>
+  </si>
+  <si>
+    <t>蕭柏妮</t>
+  </si>
+  <si>
+    <t>2mg10'|con:1</t>
+  </si>
+  <si>
+    <t>keto*3</t>
+  </si>
+  <si>
     <t>32</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>盧xx</t>
   </si>
   <si>
@@ -71,9 +153,6 @@
     <t>3234567</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>79</t>
   </si>
   <si>
@@ -83,9 +162,6 @@
     <t xml:space="preserve"> right hemicolectomy (lap...</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>王曼玲</t>
   </si>
   <si>
@@ -122,6 +198,30 @@
     <t xml:space="preserve">mar:265mg+fen:0.5mg /400ML  </t>
   </si>
   <si>
+    <t>(8-8)</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>卓xx</t>
+  </si>
+  <si>
+    <t>09PW_05_01</t>
+  </si>
+  <si>
+    <t>5234567</t>
+  </si>
+  <si>
+    <t>Encounter for supervision of normal...</t>
+  </si>
+  <si>
+    <t>Cesarean section</t>
+  </si>
+  <si>
+    <t>林怡萱</t>
+  </si>
+  <si>
     <t>painless</t>
   </si>
   <si>
@@ -134,42 +234,290 @@
     <t>6234567</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>28</t>
   </si>
   <si>
     <t>pregnancy</t>
   </si>
   <si>
-    <t>林怡萱</t>
-  </si>
-  <si>
     <t>PIB:8ml/60min|     5ml|15'|80/4h</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>789</t>
-  </si>
-  <si>
-    <t>456</t>
+    <t>17</t>
+  </si>
+  <si>
+    <t>黃xx</t>
+  </si>
+  <si>
+    <t>08B_15_01</t>
+  </si>
+  <si>
+    <t>7234567</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>Thymic tumor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right VATs </t>
+  </si>
+  <si>
+    <t>2mg10'</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Cre</t>
+  </si>
+  <si>
+    <t>個人史</t>
+  </si>
+  <si>
+    <t>藥物過敏</t>
+  </si>
+  <si>
+    <t>長期使用opioids</t>
+  </si>
+  <si>
+    <t>使用原因</t>
+  </si>
+  <si>
+    <t>剖腹產：胎次</t>
+  </si>
+  <si>
+    <t>減痛分娩：胎次</t>
+  </si>
+  <si>
+    <t>其他</t>
+  </si>
+  <si>
+    <t>麻醉結束時間</t>
+  </si>
+  <si>
+    <t>預計使用期間</t>
+  </si>
+  <si>
+    <t>已知用藥-Zfran</t>
+  </si>
+  <si>
+    <t>已知用藥-OR</t>
+  </si>
+  <si>
+    <t>已知用藥-POR</t>
+  </si>
+  <si>
+    <t>臨時上機</t>
+  </si>
+  <si>
+    <t>臨時上機-時間</t>
+  </si>
+  <si>
+    <t>臨時上機-地點</t>
+  </si>
+  <si>
+    <t>鎖牌號碼</t>
+  </si>
+  <si>
+    <t>止痛方式</t>
+  </si>
+  <si>
+    <t>止痛藥物</t>
+  </si>
+  <si>
+    <t>機器設定-Loading dose</t>
+  </si>
+  <si>
+    <t>機器設定-PCA dose</t>
+  </si>
+  <si>
+    <t>機器設定-Infusion dose</t>
+  </si>
+  <si>
+    <t>機器設定-Lock-out interval</t>
+  </si>
+  <si>
+    <t>機器設定-4-hr limit</t>
+  </si>
+  <si>
+    <t>位置</t>
+  </si>
+  <si>
+    <t>fix</t>
+  </si>
+  <si>
+    <t>施打者</t>
+  </si>
+  <si>
+    <t>下床時間</t>
+  </si>
+  <si>
+    <t>排氣時間</t>
+  </si>
+  <si>
+    <t>胎次</t>
+  </si>
+  <si>
+    <t>PFE(PCA)</t>
+  </si>
+  <si>
+    <t>病人狀況-日期</t>
+  </si>
+  <si>
+    <t>病人狀況-時間</t>
+  </si>
+  <si>
+    <t>已輸液量</t>
+  </si>
+  <si>
+    <t>有效次數</t>
+  </si>
+  <si>
+    <t>請求次數</t>
+  </si>
+  <si>
+    <t>VAS(動)</t>
+  </si>
+  <si>
+    <t>VAS(靜)</t>
+  </si>
+  <si>
+    <t>VAS(宮縮)</t>
+  </si>
+  <si>
+    <t>頭暈</t>
+  </si>
+  <si>
+    <t>噁心</t>
+  </si>
+  <si>
+    <t>嘔吐</t>
+  </si>
+  <si>
+    <t>癢疹</t>
+  </si>
+  <si>
+    <t>嗜睡</t>
+  </si>
+  <si>
+    <t>難尿</t>
+  </si>
+  <si>
+    <t>頭痛</t>
+  </si>
+  <si>
+    <t>腳麻</t>
+  </si>
+  <si>
+    <t>處置</t>
+  </si>
+  <si>
+    <t>EA導管</t>
+  </si>
+  <si>
+    <t>衛教</t>
+  </si>
+  <si>
+    <t>其他交班事項</t>
+  </si>
+  <si>
+    <t>備袋</t>
+  </si>
+  <si>
+    <t>備袋狀況</t>
+  </si>
+  <si>
+    <t>U1126</t>
+  </si>
+  <si>
+    <t>用藥資料單完成</t>
+  </si>
+  <si>
+    <t>00:00</t>
+  </si>
+  <si>
+    <t>4mg</t>
+  </si>
+  <si>
+    <t>無</t>
+  </si>
+  <si>
+    <t>未確認</t>
+  </si>
+  <si>
+    <t>10 月 31 日</t>
+  </si>
+  <si>
+    <t>15 點 12 分</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>無滲濕</t>
+  </si>
+  <si>
+    <t>16 點 3 分</t>
+  </si>
+  <si>
+    <t>沈xx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-11-21 00:15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-11-26 00:15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCA同意書確認</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-11-21 00:15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-11-21 至 2017-11-26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-11-21 至 2017-11-26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-11-21 至 2017-11-26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-11-21 至 2017-11-26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-11-21 至 2017-11-26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -194,14 +542,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -526,11 +886,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="SheetJS"/>
-  <dimension ref="A1:N5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="personal information"/>
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +940,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -585,75 +951,75 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s">
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>33</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
         <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
       </c>
       <c r="M3" t="s">
         <v>35</v>
@@ -662,15 +1028,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>38</v>
@@ -682,19 +1048,19 @@
         <v>40</v>
       </c>
       <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
         <v>41</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>42</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>43</v>
       </c>
-      <c r="J4" t="s">
-        <v>37</v>
-      </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="L4" t="s">
         <v>44</v>
@@ -703,53 +1069,1540 @@
         <v>45</v>
       </c>
       <c r="N4" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>46</v>
       </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" t="s">
         <v>16</v>
       </c>
-      <c r="M5" t="s">
-        <v>14</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="L8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" t="s">
+        <v>78</v>
+      </c>
+      <c r="N8" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="form"/>
+  <dimension ref="A1:BM7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="36" width="11" style="2"/>
+    <col min="37" max="38" width="16.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11" style="2"/>
+    <col min="40" max="40" width="16.125" style="2" customWidth="1"/>
+    <col min="41" max="64" width="11" style="2"/>
+    <col min="65" max="65" width="19.625" style="2" customWidth="1"/>
+    <col min="66" max="16384" width="11" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BI2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL2" s="2">
+        <v>111</v>
+      </c>
+      <c r="BM2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AV3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AW3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AX3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BC3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BE3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BI3" s="2">
+        <v>234567</v>
+      </c>
+      <c r="BJ3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL3" s="2">
+        <v>2</v>
+      </c>
+      <c r="BM3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AR4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AV4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AW4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AX4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BC4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BE4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BI4" s="2">
+        <v>345678</v>
+      </c>
+      <c r="BJ4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL4" s="2">
+        <v>333</v>
+      </c>
+      <c r="BM4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AQ5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AR5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AV5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AW5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AX5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BC5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BE5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BI5" s="2">
+        <v>456789</v>
+      </c>
+      <c r="BJ5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL5" s="2">
+        <v>444</v>
+      </c>
+      <c r="BM5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AN6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP6" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AQ6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AR6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AV6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AW6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AX6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BC6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BE6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BI6" s="2">
+        <v>13579</v>
+      </c>
+      <c r="BJ6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL6" s="2">
+        <v>5555</v>
+      </c>
+      <c r="BM6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AN7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AQ7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AR7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AV7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AW7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AX7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BC7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BE7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BI7" s="2">
+        <v>246810</v>
+      </c>
+      <c r="BJ7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL7" s="2">
+        <v>6666</v>
+      </c>
+      <c r="BM7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>